<commit_message>
Migrate shipment fields to camelCase
</commit_message>
<xml_diff>
--- a/src/public/sample_create_orders.xlsx
+++ b/src/public/sample_create_orders.xlsx
@@ -8,12 +8,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>orderName</t>
   </si>
   <si>
-    <t>order_date</t>
+    <t>orderKey</t>
+  </si>
+  <si>
+    <t>orderId</t>
+  </si>
+  <si>
+    <t>orderGid</t>
+  </si>
+  <si>
+    <t>orderDate</t>
   </si>
   <si>
     <t>fullName</t>
@@ -43,22 +52,34 @@
     <t>pinCode</t>
   </si>
   <si>
-    <t>totalPrice</t>
-  </si>
-  <si>
-    <t>financialStatus</t>
-  </si>
-  <si>
-    <t>invoice_value</t>
-  </si>
-  <si>
-    <t>content_and_quantity</t>
+    <t>paymentStatus</t>
+  </si>
+  <si>
+    <t>invoiceValue</t>
+  </si>
+  <si>
+    <t>productDescription</t>
+  </si>
+  <si>
+    <t>fulfillmentCenter</t>
+  </si>
+  <si>
+    <t>fulfillmentStatus</t>
+  </si>
+  <si>
+    <t>weightKg</t>
+  </si>
+  <si>
+    <t>courierType</t>
   </si>
   <si>
     <t>O000001</t>
   </si>
   <si>
-    <t>2026-02-04</t>
+    <t/>
+  </si>
+  <si>
+    <t>08-02-2026</t>
   </si>
   <si>
     <t>Navneet Sinha</t>
@@ -70,9 +91,6 @@
     <t>9815582923</t>
   </si>
   <si>
-    <t>0981558292</t>
-  </si>
-  <si>
     <t>P No.-90B, Sector-18</t>
   </si>
   <si>
@@ -82,19 +100,28 @@
     <t>Gurugram</t>
   </si>
   <si>
-    <t>Haryana</t>
+    <t>HARYANA</t>
   </si>
   <si>
     <t>122001</t>
   </si>
   <si>
+    <t>paid</t>
+  </si>
+  <si>
     <t>499.00</t>
   </si>
   <si>
-    <t>paid</t>
-  </si>
-  <si>
     <t>T-Shirt x1</t>
+  </si>
+  <si>
+    <t>unfulfilled</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>Z- Express</t>
   </si>
 </sst>
 </file>
@@ -109,21 +136,9 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="1">
     <fill>
       <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD1FAE5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5E7EB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,109 +153,143 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="1">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="1">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="1">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="1">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="1">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>